<commit_message>
Prduct image in import, upload image, design, image path
</commit_message>
<xml_diff>
--- a/GoosEnterprise.Model/DBScript/Pladis 2020 Test.xlsx
+++ b/GoosEnterprise.Model/DBScript/Pladis 2020 Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GoodsEnterprise1\GoosEnterprise.Model\DBScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF99C86-71C9-4FC2-BBD0-1B0782063D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1964ABF5-3451-469C-860D-9082D5AE1830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Brand</t>
   </si>
@@ -137,6 +137,21 @@
   </si>
   <si>
     <t>Pladis1</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>E:\ProjectImage\DownloadImages\test1.png</t>
+  </si>
+  <si>
+    <t>E:\ProjectImage\DownloadImages\test2.png</t>
+  </si>
+  <si>
+    <t>E:\ProjectImage\DownloadImages\test3.png</t>
+  </si>
+  <si>
+    <t>E:\ProjectImage\DownloadImages\test4.png</t>
   </si>
 </sst>
 </file>
@@ -519,7 +534,7 @@
   <dimension ref="A1:BR326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,9 +559,10 @@
     <col min="22" max="23" width="14.77734375" style="6" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15.109375" style="8" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -637,8 +653,11 @@
       <c r="AD1" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE1" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>11172</v>
       </c>
@@ -652,7 +671,7 @@
         <v>5000118001142</v>
       </c>
       <c r="E2" s="2">
-        <v>5000129011835</v>
+        <v>5009179615835</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -729,8 +748,11 @@
       <c r="AD2" s="11">
         <v>46003</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>13027</v>
       </c>
@@ -744,7 +766,7 @@
         <v>5000118001143</v>
       </c>
       <c r="E3" s="2">
-        <v>5000129011836</v>
+        <v>5009179615836</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -818,8 +840,11 @@
       <c r="AD3" s="11">
         <v>46003</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>34763</v>
       </c>
@@ -833,7 +858,7 @@
         <v>5000118001144</v>
       </c>
       <c r="E4" s="2">
-        <v>5000129011837</v>
+        <v>5009179615837</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -907,8 +932,11 @@
       <c r="AD4" s="11">
         <v>46003</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45890</v>
       </c>
@@ -922,7 +950,7 @@
         <v>5000118001145</v>
       </c>
       <c r="E5" s="2">
-        <v>5000129011838</v>
+        <v>5009179615838</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -996,48 +1024,51 @@
       <c r="AD5" s="11">
         <v>46003</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="Y6" s="1"/>
       <c r="AD6" s="11"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="Y7" s="1"/>
       <c r="AD7" s="11"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="Y8" s="1"/>
       <c r="AD8" s="11"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="Y9" s="1"/>
       <c r="AD9" s="11"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="Y10" s="1"/>
       <c r="AD10" s="11"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="Y11" s="1"/>
       <c r="AD11" s="11"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="Y12" s="1"/>
       <c r="AD12" s="11"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="Y13" s="1"/>
       <c r="AD13" s="11"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="Y14" s="1"/>
       <c r="AD14" s="11"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="Y15" s="1"/>
       <c r="AD15" s="11"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="Y16" s="1"/>
       <c r="AD16" s="11"/>
     </row>

</xml_diff>